<commit_message>
UPL: Updated initial data files
</commit_message>
<xml_diff>
--- a/data/Cebu_Weather_Tourist.xlsx
+++ b/data/Cebu_Weather_Tourist.xlsx
@@ -143,7 +143,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,7 +152,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="11"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -167,42 +173,42 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -216,26 +222,26 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -252,58 +258,58 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="17" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="17" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="3" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="17" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="17" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -323,6 +329,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffffff00"/>
     </indexedColors>
@@ -531,17 +538,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -569,10 +576,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -820,12 +827,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1112,7 +1119,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1140,10 +1147,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1880,15 +1887,15 @@
         <v>10</v>
       </c>
       <c r="D22" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E22" s="4">
         <f>B22/SUM(B22:D22)</f>
-        <v>0.6071428571428571</v>
+        <v>0.5666666666666667</v>
       </c>
       <c r="F22" s="4">
         <f>SUM(C22:D22)/SUM(B22:D22)</f>
-        <v>0.3928571428571428</v>
+        <v>0.4333333333333333</v>
       </c>
     </row>
     <row r="23" ht="17" customHeight="1">

</xml_diff>